<commit_message>
consensus tracker v1 done
</commit_message>
<xml_diff>
--- a/current_games.xlsx
+++ b/current_games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>year</t>
   </si>
@@ -91,22 +91,70 @@
     <t>ratings_2k</t>
   </si>
   <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>Houston</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>GoldenState</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>LAClippers</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>LALakers</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>NewOrleans</t>
+  </si>
+  <si>
+    <t>SanAntonio</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
     <t>Denver</t>
   </si>
   <si>
-    <t>Memphis</t>
-  </si>
-  <si>
-    <t>Milwaukee</t>
-  </si>
-  <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>Sacramento</t>
-  </si>
-  <si>
-    <t>Washington</t>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Miami</t>
   </si>
 </sst>
 </file>
@@ -464,7 +512,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -555,61 +603,61 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>233.5</v>
+        <v>220</v>
       </c>
       <c r="E2">
-        <v>12785473.5</v>
+        <v>9117527.5</v>
       </c>
       <c r="F2">
-        <v>117.6166666666667</v>
+        <v>114.7567567567567</v>
       </c>
       <c r="G2">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="K2">
-        <v>98.37825396825396</v>
+        <v>97.09594594594594</v>
       </c>
       <c r="L2">
-        <v>118.6661507936508</v>
+        <v>116.95</v>
       </c>
       <c r="M2">
-        <v>114.220992063492</v>
+        <v>114.1621621621621</v>
       </c>
       <c r="N2">
-        <v>77.74273809523811</v>
+        <v>74.91486486486487</v>
       </c>
       <c r="O2">
-        <v>0.4144996031746032</v>
+        <v>0.3842567567567567</v>
       </c>
       <c r="P2">
-        <v>0.6077579365079365</v>
+        <v>0.5697972972972976</v>
       </c>
       <c r="Q2">
-        <v>0.2636218253968253</v>
+        <v>0.2595270270270271</v>
       </c>
       <c r="R2">
-        <v>12.47765873015873</v>
+        <v>11.42162162162162</v>
       </c>
       <c r="S2">
-        <v>11.71825396825397</v>
+        <v>12.33918918918919</v>
       </c>
       <c r="T2">
-        <v>0.2019988095238095</v>
+        <v>0.2160608108108108</v>
       </c>
       <c r="U2">
-        <v>1.03444737613603</v>
+        <v>1.00929425467684</v>
       </c>
       <c r="V2">
-        <v>1.05412130150422</v>
+        <v>0.9803899256330547</v>
       </c>
       <c r="W2">
-        <v>10.57831897349203</v>
+        <v>12.13290480795492</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -620,61 +668,61 @@
         <v>2023</v>
       </c>
       <c r="D3">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="E3">
-        <v>8027431</v>
+        <v>29061741</v>
       </c>
       <c r="F3">
-        <v>116.8180672268907</v>
+        <v>113.6347597597598</v>
       </c>
       <c r="G3">
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="K3">
-        <v>100.6290336134454</v>
+        <v>100.7531531531531</v>
       </c>
       <c r="L3">
-        <v>115.6167647058824</v>
+        <v>111.477515015015</v>
       </c>
       <c r="M3">
-        <v>112.8309663865546</v>
+        <v>115.6541666666667</v>
       </c>
       <c r="N3">
-        <v>77.34672268907562</v>
+        <v>76.00581831831832</v>
       </c>
       <c r="O3">
-        <v>0.3932714285714285</v>
+        <v>0.3515146396396396</v>
       </c>
       <c r="P3">
-        <v>0.5809327731092437</v>
+        <v>0.5597248498498499</v>
       </c>
       <c r="Q3">
-        <v>0.2823294117647058</v>
+        <v>0.2680480480480481</v>
       </c>
       <c r="R3">
-        <v>12.2436974789916</v>
+        <v>12.04283033033033</v>
       </c>
       <c r="S3">
-        <v>12.35491596638655</v>
+        <v>11.77522522522522</v>
       </c>
       <c r="T3">
-        <v>0.2120504201680672</v>
+        <v>0.2031355105105105</v>
       </c>
       <c r="U3">
-        <v>1.027423634361396</v>
+        <v>0.9994262072098483</v>
       </c>
       <c r="V3">
-        <v>1.001428288590727</v>
+        <v>1.010220801718564</v>
       </c>
       <c r="W3">
-        <v>11.85607454599895</v>
+        <v>11.52935259639596</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -685,61 +733,581 @@
         <v>2023</v>
       </c>
       <c r="D4">
-        <v>226.5</v>
+        <v>222.5</v>
       </c>
       <c r="E4">
-        <v>9248915.5</v>
+        <v>27144508.5</v>
       </c>
       <c r="F4">
-        <v>112.4444015444015</v>
+        <v>112.4966216216216</v>
       </c>
       <c r="G4">
-        <v>6.5</v>
+        <v>4</v>
       </c>
       <c r="H4" t="s">
         <v>27</v>
       </c>
       <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4">
+        <v>96.98532282282282</v>
+      </c>
+      <c r="L4">
+        <v>114.5106606606607</v>
+      </c>
+      <c r="M4">
+        <v>112.3473348348348</v>
+      </c>
+      <c r="N4">
+        <v>78.34399399399399</v>
+      </c>
+      <c r="O4">
+        <v>0.3512563813813814</v>
+      </c>
+      <c r="P4">
+        <v>0.5879534534534534</v>
+      </c>
+      <c r="Q4">
+        <v>0.2684493243243243</v>
+      </c>
+      <c r="R4">
+        <v>12.44913663663664</v>
+      </c>
+      <c r="S4">
+        <v>13.17030780780781</v>
+      </c>
+      <c r="T4">
+        <v>0.2090797672672673</v>
+      </c>
+      <c r="U4">
+        <v>0.9894161971998383</v>
+      </c>
+      <c r="V4">
+        <v>1.035599661109865</v>
+      </c>
+      <c r="W4">
+        <v>10.62406666067776</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2023</v>
+      </c>
+      <c r="D5">
+        <v>232.5</v>
+      </c>
+      <c r="E5">
+        <v>7783769.5</v>
+      </c>
+      <c r="F5">
+        <v>113.341966966967</v>
+      </c>
+      <c r="G5">
+        <v>1.5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5">
+        <v>98.48930180180179</v>
+      </c>
+      <c r="L5">
+        <v>114.8377627627627</v>
+      </c>
+      <c r="M5">
+        <v>115.0150900900901</v>
+      </c>
+      <c r="N5">
+        <v>74.83956456456457</v>
+      </c>
+      <c r="O5">
+        <v>0.4010623123123123</v>
+      </c>
+      <c r="P5">
+        <v>0.5685412912912914</v>
+      </c>
+      <c r="Q5">
+        <v>0.2706647897897898</v>
+      </c>
+      <c r="R5">
+        <v>11.65037537537538</v>
+      </c>
+      <c r="S5">
+        <v>14.11865615615616</v>
+      </c>
+      <c r="T5">
+        <v>0.2253213213213214</v>
+      </c>
+      <c r="U5">
+        <v>0.9968510727085924</v>
+      </c>
+      <c r="V5">
+        <v>1.067716420524253</v>
+      </c>
+      <c r="W5">
+        <v>11.50178935367807</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2023</v>
+      </c>
+      <c r="D6">
+        <v>228.5</v>
+      </c>
+      <c r="E6">
+        <v>6971269.5</v>
+      </c>
+      <c r="F6">
+        <v>114.7626984126984</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6">
+        <v>98.11813492063492</v>
+      </c>
+      <c r="L6">
+        <v>115.4142857142857</v>
+      </c>
+      <c r="M6">
+        <v>111.1048015873016</v>
+      </c>
+      <c r="N6">
+        <v>76.72206349206348</v>
+      </c>
+      <c r="O6">
+        <v>0.3725071428571429</v>
+      </c>
+      <c r="P6">
+        <v>0.5909944444444444</v>
+      </c>
+      <c r="Q6">
+        <v>0.2930142857142857</v>
+      </c>
+      <c r="R6">
+        <v>12.73468253968254</v>
+      </c>
+      <c r="S6">
+        <v>13.57638888888889</v>
+      </c>
+      <c r="T6">
+        <v>0.2215966269841269</v>
+      </c>
+      <c r="U6">
+        <v>1.009346511985034</v>
+      </c>
+      <c r="V6">
+        <v>1.001051941146769</v>
+      </c>
+      <c r="W6">
+        <v>9.932655772870952</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2023</v>
+      </c>
+      <c r="D7">
+        <v>236</v>
+      </c>
+      <c r="E7">
+        <v>12228211</v>
+      </c>
+      <c r="F7">
+        <v>113.1805555555556</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="K4">
-        <v>98.5483783783784</v>
-      </c>
-      <c r="L4">
-        <v>113.4245173745174</v>
-      </c>
-      <c r="M4">
-        <v>112.6574517374517</v>
-      </c>
-      <c r="N4">
-        <v>78.09324324324325</v>
-      </c>
-      <c r="O4">
-        <v>0.3924799227799228</v>
-      </c>
-      <c r="P4">
-        <v>0.5733806949806949</v>
-      </c>
-      <c r="Q4">
-        <v>0.2704930501930503</v>
-      </c>
-      <c r="R4">
-        <v>12.37718146718147</v>
-      </c>
-      <c r="S4">
-        <v>10.94737451737452</v>
-      </c>
-      <c r="T4">
-        <v>0.2009990347490347</v>
-      </c>
-      <c r="U4">
-        <v>0.9889569177168122</v>
-      </c>
-      <c r="V4">
-        <v>1.061338647179362</v>
-      </c>
-      <c r="W4">
-        <v>10.981174280014</v>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7">
+        <v>98.93194444444445</v>
+      </c>
+      <c r="L7">
+        <v>114.1652777777778</v>
+      </c>
+      <c r="M7">
+        <v>116.5958333333333</v>
+      </c>
+      <c r="N7">
+        <v>75.11527777777778</v>
+      </c>
+      <c r="O7">
+        <v>0.3645</v>
+      </c>
+      <c r="P7">
+        <v>0.5904444444444445</v>
+      </c>
+      <c r="Q7">
+        <v>0.2441527777777778</v>
+      </c>
+      <c r="R7">
+        <v>13.27916666666667</v>
+      </c>
+      <c r="S7">
+        <v>12.20277777777778</v>
+      </c>
+      <c r="T7">
+        <v>0.1984444444444444</v>
+      </c>
+      <c r="U7">
+        <v>0.9954314472784129</v>
+      </c>
+      <c r="V7">
+        <v>1.056064432619845</v>
+      </c>
+      <c r="W7">
+        <v>11.2517907146846</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2023</v>
+      </c>
+      <c r="D8">
+        <v>227.5</v>
+      </c>
+      <c r="E8">
+        <v>18039865.5</v>
+      </c>
+      <c r="F8">
+        <v>111.0191441441441</v>
+      </c>
+      <c r="G8">
+        <v>7.5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8">
+        <v>96.80953453453452</v>
+      </c>
+      <c r="L8">
+        <v>113.5811186186186</v>
+      </c>
+      <c r="M8">
+        <v>115.7282657657658</v>
+      </c>
+      <c r="N8">
+        <v>76.26482732732731</v>
+      </c>
+      <c r="O8">
+        <v>0.447734984984985</v>
+      </c>
+      <c r="P8">
+        <v>0.573355855855856</v>
+      </c>
+      <c r="Q8">
+        <v>0.3004279279279278</v>
+      </c>
+      <c r="R8">
+        <v>12.66126126126126</v>
+      </c>
+      <c r="S8">
+        <v>12.42927927927928</v>
+      </c>
+      <c r="T8">
+        <v>0.2202346096096096</v>
+      </c>
+      <c r="U8">
+        <v>0.9764216723319626</v>
+      </c>
+      <c r="V8">
+        <v>1.026896583993006</v>
+      </c>
+      <c r="W8">
+        <v>11.85468046490976</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2023</v>
+      </c>
+      <c r="D9">
+        <v>233</v>
+      </c>
+      <c r="E9">
+        <v>5704334</v>
+      </c>
+      <c r="F9">
+        <v>115.4943693693694</v>
+      </c>
+      <c r="G9">
+        <v>1.5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9">
+        <v>99.66302552552551</v>
+      </c>
+      <c r="L9">
+        <v>115.4558183183183</v>
+      </c>
+      <c r="M9">
+        <v>115.0661786786787</v>
+      </c>
+      <c r="N9">
+        <v>75.98453453453455</v>
+      </c>
+      <c r="O9">
+        <v>0.3620923423423424</v>
+      </c>
+      <c r="P9">
+        <v>0.6001133633633633</v>
+      </c>
+      <c r="Q9">
+        <v>0.272468093093093</v>
+      </c>
+      <c r="R9">
+        <v>13.47447447447447</v>
+      </c>
+      <c r="S9">
+        <v>12.49733483483483</v>
+      </c>
+      <c r="T9">
+        <v>0.2107308558558558</v>
+      </c>
+      <c r="U9">
+        <v>1.015781612747312</v>
+      </c>
+      <c r="V9">
+        <v>1.022725388371803</v>
+      </c>
+      <c r="W9">
+        <v>10.55135318577571</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2023</v>
+      </c>
+      <c r="D10">
+        <v>236.5</v>
+      </c>
+      <c r="E10">
+        <v>26892659.5</v>
+      </c>
+      <c r="F10">
+        <v>115.4665915915916</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10">
+        <v>100.9704204204204</v>
+      </c>
+      <c r="L10">
+        <v>113.7746246246246</v>
+      </c>
+      <c r="M10">
+        <v>114.487987987988</v>
+      </c>
+      <c r="N10">
+        <v>75.95762012012011</v>
+      </c>
+      <c r="O10">
+        <v>0.4072072072072072</v>
+      </c>
+      <c r="P10">
+        <v>0.5786854354354354</v>
+      </c>
+      <c r="Q10">
+        <v>0.233021021021021</v>
+      </c>
+      <c r="R10">
+        <v>12.49489489489489</v>
+      </c>
+      <c r="S10">
+        <v>12.52154654654655</v>
+      </c>
+      <c r="T10">
+        <v>0.2077937312312312</v>
+      </c>
+      <c r="U10">
+        <v>1.015537305115142</v>
+      </c>
+      <c r="V10">
+        <v>0.9845002794365048</v>
+      </c>
+      <c r="W10">
+        <v>10.26464892898018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2023</v>
+      </c>
+      <c r="D11">
+        <v>232.5</v>
+      </c>
+      <c r="E11">
+        <v>5780100.5</v>
+      </c>
+      <c r="F11">
+        <v>112.0161172161172</v>
+      </c>
+      <c r="G11">
+        <v>9.5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11">
+        <v>97.70673992673991</v>
+      </c>
+      <c r="L11">
+        <v>113.8320512820513</v>
+      </c>
+      <c r="M11">
+        <v>117.210695970696</v>
+      </c>
+      <c r="N11">
+        <v>75.41615384615383</v>
+      </c>
+      <c r="O11">
+        <v>0.3890912087912087</v>
+      </c>
+      <c r="P11">
+        <v>0.5751838827838828</v>
+      </c>
+      <c r="Q11">
+        <v>0.3015227106227106</v>
+      </c>
+      <c r="R11">
+        <v>12.80333333333333</v>
+      </c>
+      <c r="S11">
+        <v>11.82978021978022</v>
+      </c>
+      <c r="T11">
+        <v>0.224779304029304</v>
+      </c>
+      <c r="U11">
+        <v>0.9851901250318136</v>
+      </c>
+      <c r="V11">
+        <v>1.038595911054708</v>
+      </c>
+      <c r="W11">
+        <v>11.46643013667387</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>2023</v>
+      </c>
+      <c r="D12">
+        <v>219</v>
+      </c>
+      <c r="E12">
+        <v>18267580</v>
+      </c>
+      <c r="F12">
+        <v>109.3684210526316</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12">
+        <v>97.05963726884779</v>
+      </c>
+      <c r="L12">
+        <v>111.9332859174964</v>
+      </c>
+      <c r="M12">
+        <v>112.2169985775249</v>
+      </c>
+      <c r="N12">
+        <v>76.95874822190612</v>
+      </c>
+      <c r="O12">
+        <v>0.4120352062588905</v>
+      </c>
+      <c r="P12">
+        <v>0.5730515647226174</v>
+      </c>
+      <c r="Q12">
+        <v>0.2653641536273116</v>
+      </c>
+      <c r="R12">
+        <v>12.66995021337127</v>
+      </c>
+      <c r="S12">
+        <v>12.99615931721195</v>
+      </c>
+      <c r="T12">
+        <v>0.200503733997155</v>
+      </c>
+      <c r="U12">
+        <v>0.9619034393371292</v>
+      </c>
+      <c r="V12">
+        <v>1.098709289449174</v>
+      </c>
+      <c r="W12">
+        <v>10.56192804635218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
basic setup for spread model setup
</commit_message>
<xml_diff>
--- a/current_games.xlsx
+++ b/current_games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>year</t>
   </si>
@@ -91,28 +91,34 @@
     <t>ratings_2k</t>
   </si>
   <si>
+    <t>SanAntonio</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Dallas</t>
+  </si>
+  <si>
+    <t>GoldenState</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>NewOrleans</t>
+  </si>
+  <si>
     <t>Orlando</t>
   </si>
   <si>
-    <t>Dallas</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
-    <t>Denver</t>
-  </si>
-  <si>
-    <t>Memphis</t>
-  </si>
-  <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>LAClippers</t>
+    <t>LALakers</t>
   </si>
 </sst>
 </file>
@@ -470,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -561,64 +567,64 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>231.5</v>
+        <v>234.5</v>
       </c>
       <c r="E2">
-        <v>5795914</v>
+        <v>17253288.5</v>
       </c>
       <c r="F2">
-        <v>113.0245376955903</v>
+        <v>115.3205128205128</v>
       </c>
       <c r="G2">
-        <v>6.5</v>
+        <v>13.5</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J2">
-        <v>0.4861111111111111</v>
+        <v>0.5462304409672831</v>
       </c>
       <c r="K2">
-        <v>99.16586059743953</v>
+        <v>99.5051282051282</v>
       </c>
       <c r="L2">
-        <v>113.3929587482219</v>
+        <v>115.3269230769231</v>
       </c>
       <c r="M2">
-        <v>112.9138335704125</v>
+        <v>116.55</v>
       </c>
       <c r="N2">
-        <v>76.6512091038407</v>
+        <v>76.61538461538463</v>
       </c>
       <c r="O2">
-        <v>0.3611095305832148</v>
+        <v>0.4154102564102563</v>
       </c>
       <c r="P2">
-        <v>0.5675633001422475</v>
+        <v>0.5860769230769232</v>
       </c>
       <c r="Q2">
-        <v>0.2864342105263158</v>
+        <v>0.2534230769230769</v>
       </c>
       <c r="R2">
-        <v>12.64260312944523</v>
+        <v>12.70128205128205</v>
       </c>
       <c r="S2">
-        <v>12.03061877667141</v>
+        <v>11.8525641025641</v>
       </c>
       <c r="T2">
-        <v>0.2137290184921763</v>
+        <v>0.1952115384615385</v>
       </c>
       <c r="U2">
-        <v>0.9931857442494758</v>
+        <v>1.013361272587986</v>
       </c>
       <c r="V2">
-        <v>1.019663157391185</v>
+        <v>0.9974903451022887</v>
       </c>
       <c r="W2">
-        <v>11.52516041031066</v>
+        <v>11.12508988895773</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -629,64 +635,64 @@
         <v>2023</v>
       </c>
       <c r="D3">
-        <v>231</v>
+        <v>238.5</v>
       </c>
       <c r="E3">
-        <v>15244031</v>
+        <v>19299819</v>
       </c>
       <c r="F3">
-        <v>115.5789473684211</v>
+        <v>116.1529080675422</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J3">
-        <v>0.5533625730994152</v>
+        <v>0.5185897435897436</v>
       </c>
       <c r="K3">
-        <v>96.9736842105263</v>
+        <v>99.31041275797372</v>
       </c>
       <c r="L3">
-        <v>117.8473684210526</v>
+        <v>115.8054721701063</v>
       </c>
       <c r="M3">
-        <v>113.9381578947368</v>
+        <v>115.7099749843652</v>
       </c>
       <c r="N3">
-        <v>77.29605263157896</v>
+        <v>76.27911194496559</v>
       </c>
       <c r="O3">
-        <v>0.4868552631578947</v>
+        <v>0.3890678549093183</v>
       </c>
       <c r="P3">
-        <v>0.6008684210526316</v>
+        <v>0.5898373983739836</v>
       </c>
       <c r="Q3">
-        <v>0.2871973684210526</v>
+        <v>0.2630712945590995</v>
       </c>
       <c r="R3">
-        <v>11.46184210526316</v>
+        <v>12.4750469043152</v>
       </c>
       <c r="S3">
-        <v>11.99078947368421</v>
+        <v>12.53164477798624</v>
       </c>
       <c r="T3">
-        <v>0.2142960526315789</v>
+        <v>0.2111558786741714</v>
       </c>
       <c r="U3">
-        <v>1.015632226436037</v>
+        <v>1.020675817816715</v>
       </c>
       <c r="V3">
-        <v>1.025345459080376</v>
+        <v>1.076525518682472</v>
       </c>
       <c r="W3">
-        <v>11.70460894822567</v>
+        <v>10.68952267008545</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -697,64 +703,64 @@
         <v>2023</v>
       </c>
       <c r="D4">
-        <v>230.5</v>
+        <v>225.5</v>
       </c>
       <c r="E4">
-        <v>16854023</v>
+        <v>8276298.5</v>
       </c>
       <c r="F4">
-        <v>113.2447368421053</v>
+        <v>114.6025641025641</v>
       </c>
       <c r="G4">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="H4" t="s">
         <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J4">
-        <v>0.5060728744939271</v>
+        <v>0.5641025641025641</v>
       </c>
       <c r="K4">
-        <v>98.96046052631579</v>
+        <v>97.23846153846154</v>
       </c>
       <c r="L4">
-        <v>113.6141447368421</v>
+        <v>116.2141025641026</v>
       </c>
       <c r="M4">
-        <v>116.768552631579</v>
+        <v>113.2615384615385</v>
       </c>
       <c r="N4">
-        <v>75.13374999999999</v>
+        <v>77.02051282051281</v>
       </c>
       <c r="O4">
-        <v>0.4231138157894737</v>
+        <v>0.4216666666666667</v>
       </c>
       <c r="P4">
-        <v>0.5696565789473684</v>
+        <v>0.5883589743589743</v>
       </c>
       <c r="Q4">
-        <v>0.2794427631578947</v>
+        <v>0.3035897435897436</v>
       </c>
       <c r="R4">
-        <v>13.47730263157895</v>
+        <v>11.9051282051282</v>
       </c>
       <c r="S4">
-        <v>12.20986842105263</v>
+        <v>12.92564102564102</v>
       </c>
       <c r="T4">
-        <v>0.2152651315789474</v>
+        <v>0.2227948717948718</v>
       </c>
       <c r="U4">
-        <v>0.9951207103875682</v>
+        <v>1.007052408634131</v>
       </c>
       <c r="V4">
-        <v>0.9767622100832026</v>
+        <v>0.9661064756566271</v>
       </c>
       <c r="W4">
-        <v>10.91400706352906</v>
+        <v>10.77742982739587</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -765,64 +771,132 @@
         <v>2023</v>
       </c>
       <c r="D5">
-        <v>228</v>
+        <v>231.5</v>
       </c>
       <c r="E5">
-        <v>8164211</v>
+        <v>27155624</v>
       </c>
       <c r="F5">
-        <v>112.959805959806</v>
+        <v>113.7307692307692</v>
       </c>
       <c r="G5">
-        <v>5</v>
+        <v>6.5</v>
       </c>
       <c r="H5" t="s">
         <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J5">
-        <v>0.4618849618849619</v>
+        <v>0.5597439544807966</v>
       </c>
       <c r="K5">
-        <v>97.75814275814274</v>
+        <v>99.80512820512823</v>
       </c>
       <c r="L5">
-        <v>114.9310464310464</v>
+        <v>113.2346153846154</v>
       </c>
       <c r="M5">
-        <v>114.0732848232848</v>
+        <v>115.4423076923077</v>
       </c>
       <c r="N5">
-        <v>77.29916839916839</v>
+        <v>76.49871794871795</v>
       </c>
       <c r="O5">
-        <v>0.3751153846153847</v>
+        <v>0.4217179487179488</v>
       </c>
       <c r="P5">
-        <v>0.5934729729729731</v>
+        <v>0.5855384615384613</v>
       </c>
       <c r="Q5">
-        <v>0.2741628551628552</v>
+        <v>0.2613974358974359</v>
       </c>
       <c r="R5">
-        <v>13.38042273042273</v>
+        <v>13.76794871794872</v>
       </c>
       <c r="S5">
-        <v>11.65252945252945</v>
+        <v>11.97435897435897</v>
       </c>
       <c r="T5">
-        <v>0.2042676715176715</v>
+        <v>0.2149807692307692</v>
       </c>
       <c r="U5">
-        <v>0.9926169240756236</v>
+        <v>0.9993916452615925</v>
       </c>
       <c r="V5">
-        <v>1.030021846326244</v>
+        <v>1.055825170109766</v>
       </c>
       <c r="W5">
-        <v>10.45201563605339</v>
+        <v>11.02751638816982</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2023</v>
+      </c>
+      <c r="D6">
+        <v>241.5</v>
+      </c>
+      <c r="E6">
+        <v>31473048</v>
+      </c>
+      <c r="F6">
+        <v>117.1389466389466</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6">
+        <v>0.517094017094017</v>
+      </c>
+      <c r="K6">
+        <v>101.4100831600831</v>
+      </c>
+      <c r="L6">
+        <v>114.9733194733195</v>
+      </c>
+      <c r="M6">
+        <v>114.9518018018018</v>
+      </c>
+      <c r="N6">
+        <v>77.20772695772695</v>
+      </c>
+      <c r="O6">
+        <v>0.3840717255717255</v>
+      </c>
+      <c r="P6">
+        <v>0.5918808038808039</v>
+      </c>
+      <c r="Q6">
+        <v>0.2856933471933473</v>
+      </c>
+      <c r="R6">
+        <v>12.595841995842</v>
+      </c>
+      <c r="S6">
+        <v>11.55696465696466</v>
+      </c>
+      <c r="T6">
+        <v>0.2125571725571726</v>
+      </c>
+      <c r="U6">
+        <v>1.029340480131341</v>
+      </c>
+      <c r="V6">
+        <v>1.0033256993911</v>
+      </c>
+      <c r="W6">
+        <v>11.30656842760246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some work on spread model and start system to evaluate injuries (currently have a way to determine the players on IL at any given date
</commit_message>
<xml_diff>
--- a/current_games.xlsx
+++ b/current_games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>year</t>
   </si>
@@ -91,34 +91,52 @@
     <t>ratings_2k</t>
   </si>
   <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>Detroit</t>
+  </si>
+  <si>
+    <t>Atlanta</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>NewYork</t>
+  </si>
+  <si>
+    <t>Memphis</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Sacramento</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Milwaukee</t>
+  </si>
+  <si>
+    <t>NewOrleans</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
     <t>SanAntonio</t>
   </si>
   <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Dallas</t>
-  </si>
-  <si>
-    <t>GoldenState</t>
-  </si>
-  <si>
-    <t>Sacramento</t>
-  </si>
-  <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>Utah</t>
-  </si>
-  <si>
-    <t>NewOrleans</t>
-  </si>
-  <si>
-    <t>Orlando</t>
-  </si>
-  <si>
-    <t>LALakers</t>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>Houston</t>
   </si>
 </sst>
 </file>
@@ -476,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z6"/>
+  <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -567,64 +585,64 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>234.5</v>
+        <v>228.5</v>
       </c>
       <c r="E2">
-        <v>17253288.5</v>
+        <v>19322371</v>
       </c>
       <c r="F2">
-        <v>115.3205128205128</v>
+        <v>113.3658536585366</v>
       </c>
       <c r="G2">
-        <v>13.5</v>
+        <v>1.5</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J2">
-        <v>0.5462304409672831</v>
+        <v>0.4939024390243902</v>
       </c>
       <c r="K2">
-        <v>99.5051282051282</v>
+        <v>98.75243902439024</v>
       </c>
       <c r="L2">
-        <v>115.3269230769231</v>
+        <v>113.9414634146341</v>
       </c>
       <c r="M2">
-        <v>116.55</v>
+        <v>114.9731707317073</v>
       </c>
       <c r="N2">
-        <v>76.61538461538463</v>
+        <v>77.76707317073171</v>
       </c>
       <c r="O2">
-        <v>0.4154102564102563</v>
+        <v>0.3463536585365854</v>
       </c>
       <c r="P2">
-        <v>0.5860769230769232</v>
+        <v>0.5854634146341462</v>
       </c>
       <c r="Q2">
-        <v>0.2534230769230769</v>
+        <v>0.2659634146341464</v>
       </c>
       <c r="R2">
-        <v>12.70128205128205</v>
+        <v>12.09390243902439</v>
       </c>
       <c r="S2">
-        <v>11.8525641025641</v>
+        <v>11.74024390243903</v>
       </c>
       <c r="T2">
-        <v>0.1952115384615385</v>
+        <v>0.2083841463414634</v>
       </c>
       <c r="U2">
-        <v>1.013361272587986</v>
+        <v>0.996185005786789</v>
       </c>
       <c r="V2">
-        <v>0.9974903451022887</v>
+        <v>1.008397028021033</v>
       </c>
       <c r="W2">
-        <v>11.12508988895773</v>
+        <v>10.44546646695767</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -635,64 +653,64 @@
         <v>2023</v>
       </c>
       <c r="D3">
-        <v>238.5</v>
+        <v>232</v>
       </c>
       <c r="E3">
-        <v>19299819</v>
+        <v>5116589</v>
       </c>
       <c r="F3">
-        <v>116.1529080675422</v>
+        <v>113.2619179600887</v>
       </c>
       <c r="G3">
-        <v>1.5</v>
+        <v>6</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J3">
-        <v>0.5185897435897436</v>
+        <v>0.5340328984685195</v>
       </c>
       <c r="K3">
-        <v>99.31041275797372</v>
+        <v>100.0564024390244</v>
       </c>
       <c r="L3">
-        <v>115.8054721701063</v>
+        <v>112.7019955654102</v>
       </c>
       <c r="M3">
-        <v>115.7099749843652</v>
+        <v>116.6864745011086</v>
       </c>
       <c r="N3">
-        <v>76.27911194496559</v>
+        <v>74.14212860310421</v>
       </c>
       <c r="O3">
-        <v>0.3890678549093183</v>
+        <v>0.3745354767184035</v>
       </c>
       <c r="P3">
-        <v>0.5898373983739836</v>
+        <v>0.57735088691796</v>
       </c>
       <c r="Q3">
-        <v>0.2630712945590995</v>
+        <v>0.2991524390243901</v>
       </c>
       <c r="R3">
-        <v>12.4750469043152</v>
+        <v>13.11798780487805</v>
       </c>
       <c r="S3">
-        <v>12.53164477798624</v>
+        <v>12.46804323725055</v>
       </c>
       <c r="T3">
-        <v>0.2111558786741714</v>
+        <v>0.2282720343680709</v>
       </c>
       <c r="U3">
-        <v>1.020675817816715</v>
+        <v>0.9952716868197601</v>
       </c>
       <c r="V3">
-        <v>1.076525518682472</v>
+        <v>1.002093628025482</v>
       </c>
       <c r="W3">
-        <v>10.68952267008545</v>
+        <v>11.26227294766619</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -703,64 +721,64 @@
         <v>2023</v>
       </c>
       <c r="D4">
-        <v>225.5</v>
+        <v>228.5</v>
       </c>
       <c r="E4">
-        <v>8276298.5</v>
+        <v>7962208.5</v>
       </c>
       <c r="F4">
-        <v>114.6025641025641</v>
+        <v>113.8125</v>
       </c>
       <c r="G4">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="H4" t="s">
         <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J4">
-        <v>0.5641025641025641</v>
+        <v>0.55</v>
       </c>
       <c r="K4">
-        <v>97.23846153846154</v>
+        <v>99.68500000000002</v>
       </c>
       <c r="L4">
-        <v>116.2141025641026</v>
+        <v>112.94375</v>
       </c>
       <c r="M4">
-        <v>113.2615384615385</v>
+        <v>112.8325</v>
       </c>
       <c r="N4">
-        <v>77.02051282051281</v>
+        <v>76.79749999999999</v>
       </c>
       <c r="O4">
-        <v>0.4216666666666667</v>
+        <v>0.381875</v>
       </c>
       <c r="P4">
-        <v>0.5883589743589743</v>
+        <v>0.5632999999999999</v>
       </c>
       <c r="Q4">
-        <v>0.3035897435897436</v>
+        <v>0.25385</v>
       </c>
       <c r="R4">
-        <v>11.9051282051282</v>
+        <v>11.83375</v>
       </c>
       <c r="S4">
-        <v>12.92564102564102</v>
+        <v>11.53125</v>
       </c>
       <c r="T4">
-        <v>0.2227948717948718</v>
+        <v>0.19944375</v>
       </c>
       <c r="U4">
-        <v>1.007052408634131</v>
+        <v>1.000109841827768</v>
       </c>
       <c r="V4">
-        <v>0.9661064756566271</v>
+        <v>0.9808954594845883</v>
       </c>
       <c r="W4">
-        <v>10.77742982739587</v>
+        <v>10.6887837355695</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -771,64 +789,64 @@
         <v>2023</v>
       </c>
       <c r="D5">
-        <v>231.5</v>
+        <v>231</v>
       </c>
       <c r="E5">
-        <v>27155624</v>
+        <v>12984634.5</v>
       </c>
       <c r="F5">
-        <v>113.7307692307692</v>
+        <v>117.9634146341463</v>
       </c>
       <c r="G5">
-        <v>6.5</v>
+        <v>9.5</v>
       </c>
       <c r="H5" t="s">
         <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J5">
-        <v>0.5597439544807966</v>
+        <v>0.5490931832395247</v>
       </c>
       <c r="K5">
-        <v>99.80512820512823</v>
+        <v>99.15731707317073</v>
       </c>
       <c r="L5">
-        <v>113.2346153846154</v>
+        <v>117.6634146341463</v>
       </c>
       <c r="M5">
-        <v>115.4423076923077</v>
+        <v>112.4219512195122</v>
       </c>
       <c r="N5">
-        <v>76.49871794871795</v>
+        <v>77.84146341463415</v>
       </c>
       <c r="O5">
-        <v>0.4217179487179488</v>
+        <v>0.410890243902439</v>
       </c>
       <c r="P5">
-        <v>0.5855384615384613</v>
+        <v>0.5952073170731706</v>
       </c>
       <c r="Q5">
-        <v>0.2613974358974359</v>
+        <v>0.2806463414634147</v>
       </c>
       <c r="R5">
-        <v>13.76794871794872</v>
+        <v>12.13292682926829</v>
       </c>
       <c r="S5">
-        <v>11.97435897435897</v>
+        <v>12.44390243902439</v>
       </c>
       <c r="T5">
-        <v>0.2149807692307692</v>
+        <v>0.2097560975609756</v>
       </c>
       <c r="U5">
-        <v>0.9993916452615925</v>
+        <v>1.036585365853659</v>
       </c>
       <c r="V5">
-        <v>1.055825170109766</v>
+        <v>0.9932591518117657</v>
       </c>
       <c r="W5">
-        <v>11.02751638816982</v>
+        <v>10.05097842903586</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -839,64 +857,268 @@
         <v>2023</v>
       </c>
       <c r="D6">
-        <v>241.5</v>
+        <v>226</v>
       </c>
       <c r="E6">
-        <v>31473048</v>
+        <v>9262082.5</v>
       </c>
       <c r="F6">
-        <v>117.1389466389466</v>
+        <v>114.8048780487805</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>4.5</v>
       </c>
       <c r="H6" t="s">
         <v>29</v>
       </c>
       <c r="I6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J6">
-        <v>0.517094017094017</v>
+        <v>0.4875</v>
       </c>
       <c r="K6">
-        <v>101.4100831600831</v>
+        <v>98.6731707317073</v>
       </c>
       <c r="L6">
-        <v>114.9733194733195</v>
+        <v>115.620731707317</v>
       </c>
       <c r="M6">
-        <v>114.9518018018018</v>
+        <v>114.1219512195122</v>
       </c>
       <c r="N6">
-        <v>77.20772695772695</v>
+        <v>74.58902439024391</v>
       </c>
       <c r="O6">
-        <v>0.3840717255717255</v>
+        <v>0.4136585365853658</v>
       </c>
       <c r="P6">
-        <v>0.5918808038808039</v>
+        <v>0.5721585365853659</v>
       </c>
       <c r="Q6">
-        <v>0.2856933471933473</v>
+        <v>0.2745487804878048</v>
       </c>
       <c r="R6">
-        <v>12.595841995842</v>
+        <v>11.76219512195122</v>
       </c>
       <c r="S6">
-        <v>11.55696465696466</v>
+        <v>12.29634146341463</v>
       </c>
       <c r="T6">
-        <v>0.2125571725571726</v>
+        <v>0.2201646341463414</v>
       </c>
       <c r="U6">
-        <v>1.029340480131341</v>
+        <v>1.008830211324961</v>
       </c>
       <c r="V6">
-        <v>1.0033256993911</v>
+        <v>0.9957977902620151</v>
       </c>
       <c r="W6">
-        <v>11.30656842760246</v>
+        <v>11.98146739930713</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2023</v>
+      </c>
+      <c r="D7">
+        <v>238.5</v>
+      </c>
+      <c r="E7">
+        <v>9992204.5</v>
+      </c>
+      <c r="F7">
+        <v>114.1993902439024</v>
+      </c>
+      <c r="G7">
+        <v>13.5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7">
+        <v>0.5317139001349528</v>
+      </c>
+      <c r="K7">
+        <v>100.4958231707317</v>
+      </c>
+      <c r="L7">
+        <v>113.29875</v>
+      </c>
+      <c r="M7">
+        <v>115.0175</v>
+      </c>
+      <c r="N7">
+        <v>75.95158536585365</v>
+      </c>
+      <c r="O7">
+        <v>0.353910975609756</v>
+      </c>
+      <c r="P7">
+        <v>0.5622545731707318</v>
+      </c>
+      <c r="Q7">
+        <v>0.2565567073170731</v>
+      </c>
+      <c r="R7">
+        <v>12.55484756097561</v>
+      </c>
+      <c r="S7">
+        <v>12.25079268292683</v>
+      </c>
+      <c r="T7">
+        <v>0.1932905487804878</v>
+      </c>
+      <c r="U7">
+        <v>1.003509580350636</v>
+      </c>
+      <c r="V7">
+        <v>1.046319236921261</v>
+      </c>
+      <c r="W7">
+        <v>11.35277984872319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2023</v>
+      </c>
+      <c r="D8">
+        <v>226.5</v>
+      </c>
+      <c r="E8">
+        <v>6049076.5</v>
+      </c>
+      <c r="F8">
+        <v>114.9244047619048</v>
+      </c>
+      <c r="G8">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8">
+        <v>0.4817073170731707</v>
+      </c>
+      <c r="K8">
+        <v>97.29541666666665</v>
+      </c>
+      <c r="L8">
+        <v>117.3911904761905</v>
+      </c>
+      <c r="M8">
+        <v>114.871369047619</v>
+      </c>
+      <c r="N8">
+        <v>76.4417261904762</v>
+      </c>
+      <c r="O8">
+        <v>0.3649839285714286</v>
+      </c>
+      <c r="P8">
+        <v>0.590007142857143</v>
+      </c>
+      <c r="Q8">
+        <v>0.2486589285714286</v>
+      </c>
+      <c r="R8">
+        <v>12.44607142857143</v>
+      </c>
+      <c r="S8">
+        <v>12.24357142857143</v>
+      </c>
+      <c r="T8">
+        <v>0.2096875000000001</v>
+      </c>
+      <c r="U8">
+        <v>1.009880533935894</v>
+      </c>
+      <c r="V8">
+        <v>0.991124236836904</v>
+      </c>
+      <c r="W8">
+        <v>11.34684067436913</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2023</v>
+      </c>
+      <c r="D9">
+        <v>236.5</v>
+      </c>
+      <c r="E9">
+        <v>18084349.5</v>
+      </c>
+      <c r="F9">
+        <v>113.9349358974359</v>
+      </c>
+      <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9">
+        <v>0.4743421052631579</v>
+      </c>
+      <c r="K9">
+        <v>99.6941346153846</v>
+      </c>
+      <c r="L9">
+        <v>113.7744871794872</v>
+      </c>
+      <c r="M9">
+        <v>116.4991666666667</v>
+      </c>
+      <c r="N9">
+        <v>76.89932692307693</v>
+      </c>
+      <c r="O9">
+        <v>0.4110048076923076</v>
+      </c>
+      <c r="P9">
+        <v>0.5767176282051283</v>
+      </c>
+      <c r="Q9">
+        <v>0.2881881410256409</v>
+      </c>
+      <c r="R9">
+        <v>13.24182692307692</v>
+      </c>
+      <c r="S9">
+        <v>12.29208333333333</v>
+      </c>
+      <c r="T9">
+        <v>0.2205663461538462</v>
+      </c>
+      <c r="U9">
+        <v>1.00118572844847</v>
+      </c>
+      <c r="V9">
+        <v>1.028856924773938</v>
+      </c>
+      <c r="W9">
+        <v>11.25332596191566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progress working on injury model and automatic tweet generator
</commit_message>
<xml_diff>
--- a/current_games.xlsx
+++ b/current_games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>year</t>
   </si>
@@ -91,52 +91,46 @@
     <t>ratings_2k</t>
   </si>
   <si>
-    <t>Washington</t>
-  </si>
-  <si>
-    <t>Detroit</t>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Portland</t>
+  </si>
+  <si>
+    <t>Milwaukee</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Memphis</t>
   </si>
   <si>
     <t>Atlanta</t>
   </si>
   <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>NewYork</t>
-  </si>
-  <si>
-    <t>Memphis</t>
-  </si>
-  <si>
-    <t>Denver</t>
-  </si>
-  <si>
-    <t>Sacramento</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
-  </si>
-  <si>
-    <t>Milwaukee</t>
-  </si>
-  <si>
-    <t>NewOrleans</t>
-  </si>
-  <si>
-    <t>Indiana</t>
-  </si>
-  <si>
-    <t>SanAntonio</t>
-  </si>
-  <si>
-    <t>Phoenix</t>
-  </si>
-  <si>
-    <t>Houston</t>
+    <t>Cleveland</t>
+  </si>
+  <si>
+    <t>Philadelphia</t>
+  </si>
+  <si>
+    <t>Dallas</t>
   </si>
 </sst>
 </file>
@@ -494,7 +488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z9"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -585,64 +579,64 @@
         <v>2023</v>
       </c>
       <c r="D2">
-        <v>228.5</v>
+        <v>214</v>
       </c>
       <c r="E2">
-        <v>19322371</v>
+        <v>18057017.5</v>
       </c>
       <c r="F2">
-        <v>113.3658536585366</v>
+        <v>110.4670542635659</v>
       </c>
       <c r="G2">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2">
-        <v>0.4939024390243902</v>
+        <v>0.4825581395348837</v>
       </c>
       <c r="K2">
-        <v>98.75243902439024</v>
+        <v>97.57057032115171</v>
       </c>
       <c r="L2">
-        <v>113.9414634146341</v>
+        <v>112.355869324474</v>
       </c>
       <c r="M2">
-        <v>114.9731707317073</v>
+        <v>111.7495016611296</v>
       </c>
       <c r="N2">
-        <v>77.76707317073171</v>
+        <v>77.59429678848284</v>
       </c>
       <c r="O2">
-        <v>0.3463536585365854</v>
+        <v>0.4276461794019933</v>
       </c>
       <c r="P2">
-        <v>0.5854634146341462</v>
+        <v>0.5635830564784052</v>
       </c>
       <c r="Q2">
-        <v>0.2659634146341464</v>
+        <v>0.2603803986710964</v>
       </c>
       <c r="R2">
-        <v>12.09390243902439</v>
+        <v>12.2593853820598</v>
       </c>
       <c r="S2">
-        <v>11.74024390243903</v>
+        <v>12.54111295681063</v>
       </c>
       <c r="T2">
-        <v>0.2083841463414634</v>
+        <v>0.1967003045404208</v>
       </c>
       <c r="U2">
-        <v>0.996185005786789</v>
+        <v>0.9698600023140114</v>
       </c>
       <c r="V2">
-        <v>1.008397028021033</v>
+        <v>0.9777592346727895</v>
       </c>
       <c r="W2">
-        <v>10.44546646695767</v>
+        <v>10.08080801654114</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -656,61 +650,61 @@
         <v>232</v>
       </c>
       <c r="E3">
-        <v>5116589</v>
+        <v>12877208</v>
       </c>
       <c r="F3">
-        <v>113.2619179600887</v>
+        <v>115.2906976744186</v>
       </c>
       <c r="G3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3">
-        <v>0.5340328984685195</v>
+        <v>0.5119115144639819</v>
       </c>
       <c r="K3">
-        <v>100.0564024390244</v>
+        <v>99.52790697674416</v>
       </c>
       <c r="L3">
-        <v>112.7019955654102</v>
+        <v>114.6802325581396</v>
       </c>
       <c r="M3">
-        <v>116.6864745011086</v>
+        <v>114.6837209302325</v>
       </c>
       <c r="N3">
-        <v>74.14212860310421</v>
+        <v>77.28604651162792</v>
       </c>
       <c r="O3">
-        <v>0.3745354767184035</v>
+        <v>0.4181279069767442</v>
       </c>
       <c r="P3">
-        <v>0.57735088691796</v>
+        <v>0.5751046511627909</v>
       </c>
       <c r="Q3">
-        <v>0.2991524390243901</v>
+        <v>0.2573372093023256</v>
       </c>
       <c r="R3">
-        <v>13.11798780487805</v>
+        <v>11.63372093023256</v>
       </c>
       <c r="S3">
-        <v>12.46804323725055</v>
+        <v>11.97674418604651</v>
       </c>
       <c r="T3">
-        <v>0.2282720343680709</v>
+        <v>0.2032790697674418</v>
       </c>
       <c r="U3">
-        <v>0.9952716868197601</v>
+        <v>1.012209812769259</v>
       </c>
       <c r="V3">
-        <v>1.002093628025482</v>
+        <v>0.9925835767092492</v>
       </c>
       <c r="W3">
-        <v>11.26227294766619</v>
+        <v>11.14284725284174</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -721,64 +715,64 @@
         <v>2023</v>
       </c>
       <c r="D4">
-        <v>228.5</v>
+        <v>239.5</v>
       </c>
       <c r="E4">
-        <v>7962208.5</v>
+        <v>6099441</v>
       </c>
       <c r="F4">
-        <v>113.8125</v>
+        <v>116.1349971639251</v>
       </c>
       <c r="G4">
-        <v>4.5</v>
+        <v>8.5</v>
       </c>
       <c r="H4" t="s">
         <v>27</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4">
-        <v>0.55</v>
+        <v>0.4816849816849816</v>
       </c>
       <c r="K4">
-        <v>99.68500000000002</v>
+        <v>100.5146908678389</v>
       </c>
       <c r="L4">
-        <v>112.94375</v>
+        <v>115.2277651730005</v>
       </c>
       <c r="M4">
-        <v>112.8325</v>
+        <v>112.7574021554169</v>
       </c>
       <c r="N4">
-        <v>76.79749999999999</v>
+        <v>74.57390811117412</v>
       </c>
       <c r="O4">
-        <v>0.381875</v>
+        <v>0.3940649461145773</v>
       </c>
       <c r="P4">
-        <v>0.5632999999999999</v>
+        <v>0.570916335791265</v>
       </c>
       <c r="Q4">
-        <v>0.25385</v>
+        <v>0.2701738513896766</v>
       </c>
       <c r="R4">
-        <v>11.83375</v>
+        <v>12.01554169030062</v>
       </c>
       <c r="S4">
-        <v>11.53125</v>
+        <v>12.57076006806579</v>
       </c>
       <c r="T4">
-        <v>0.19944375</v>
+        <v>0.2125994044242768</v>
       </c>
       <c r="U4">
-        <v>1.000109841827768</v>
+        <v>1.019622450956323</v>
       </c>
       <c r="V4">
-        <v>0.9808954594845883</v>
+        <v>1.031556631087341</v>
       </c>
       <c r="W4">
-        <v>10.6887837355695</v>
+        <v>11.78404703711515</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -789,64 +783,64 @@
         <v>2023</v>
       </c>
       <c r="D5">
-        <v>231</v>
+        <v>232.5</v>
       </c>
       <c r="E5">
-        <v>12984634.5</v>
+        <v>7217278</v>
       </c>
       <c r="F5">
-        <v>117.9634146341463</v>
+        <v>113.4642857142857</v>
       </c>
       <c r="G5">
-        <v>9.5</v>
+        <v>6.5</v>
       </c>
       <c r="H5" t="s">
         <v>28</v>
       </c>
       <c r="I5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J5">
-        <v>0.5490931832395247</v>
+        <v>0.5476190476190477</v>
       </c>
       <c r="K5">
-        <v>99.15731707317073</v>
+        <v>98.47142857142858</v>
       </c>
       <c r="L5">
-        <v>117.6634146341463</v>
+        <v>114.1833333333333</v>
       </c>
       <c r="M5">
-        <v>112.4219512195122</v>
+        <v>114.5785714285714</v>
       </c>
       <c r="N5">
-        <v>77.84146341463415</v>
+        <v>75.78452380952379</v>
       </c>
       <c r="O5">
-        <v>0.410890243902439</v>
+        <v>0.3484404761904761</v>
       </c>
       <c r="P5">
-        <v>0.5952073170731706</v>
+        <v>0.5589285714285714</v>
       </c>
       <c r="Q5">
-        <v>0.2806463414634147</v>
+        <v>0.263</v>
       </c>
       <c r="R5">
-        <v>12.13292682926829</v>
+        <v>10.53571428571428</v>
       </c>
       <c r="S5">
-        <v>12.44390243902439</v>
+        <v>13.70833333333333</v>
       </c>
       <c r="T5">
-        <v>0.2097560975609756</v>
+        <v>0.2185714285714286</v>
       </c>
       <c r="U5">
-        <v>1.036585365853659</v>
+        <v>0.9961745892386805</v>
       </c>
       <c r="V5">
-        <v>0.9932591518117657</v>
+        <v>1.033636535476571</v>
       </c>
       <c r="W5">
-        <v>10.05097842903586</v>
+        <v>10.46829874564268</v>
       </c>
     </row>
     <row r="6" spans="1:26">
@@ -857,64 +851,64 @@
         <v>2023</v>
       </c>
       <c r="D6">
-        <v>226</v>
+        <v>224.5</v>
       </c>
       <c r="E6">
-        <v>9262082.5</v>
+        <v>14821738.5</v>
       </c>
       <c r="F6">
-        <v>114.8048780487805</v>
+        <v>113.3139534883721</v>
       </c>
       <c r="G6">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="H6" t="s">
         <v>29</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J6">
-        <v>0.4875</v>
+        <v>0.4883720930232558</v>
       </c>
       <c r="K6">
-        <v>98.6731707317073</v>
+        <v>97.81511627906977</v>
       </c>
       <c r="L6">
-        <v>115.620731707317</v>
+        <v>114.8104651162791</v>
       </c>
       <c r="M6">
-        <v>114.1219512195122</v>
+        <v>112.5988372093023</v>
       </c>
       <c r="N6">
-        <v>74.58902439024391</v>
+        <v>76.00232558139534</v>
       </c>
       <c r="O6">
-        <v>0.4136585365853658</v>
+        <v>0.3739883720930233</v>
       </c>
       <c r="P6">
-        <v>0.5721585365853659</v>
+        <v>0.5921395348837208</v>
       </c>
       <c r="Q6">
-        <v>0.2745487804878048</v>
+        <v>0.2841046511627907</v>
       </c>
       <c r="R6">
-        <v>11.76219512195122</v>
+        <v>12.98604651162791</v>
       </c>
       <c r="S6">
-        <v>12.29634146341463</v>
+        <v>13.03255813953488</v>
       </c>
       <c r="T6">
-        <v>0.2201646341463414</v>
+        <v>0.2175813953488372</v>
       </c>
       <c r="U6">
-        <v>1.008830211324961</v>
+        <v>0.9948547277293425</v>
       </c>
       <c r="V6">
-        <v>0.9957977902620151</v>
+        <v>1.01217914971462</v>
       </c>
       <c r="W6">
-        <v>11.98146739930713</v>
+        <v>11.53275319206342</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -925,64 +919,64 @@
         <v>2023</v>
       </c>
       <c r="D7">
-        <v>238.5</v>
+        <v>235</v>
       </c>
       <c r="E7">
-        <v>9992204.5</v>
+        <v>8044823.5</v>
       </c>
       <c r="F7">
-        <v>114.1993902439024</v>
+        <v>115.5536585365854</v>
       </c>
       <c r="G7">
-        <v>13.5</v>
+        <v>5</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J7">
-        <v>0.5317139001349528</v>
+        <v>0.5889689578713969</v>
       </c>
       <c r="K7">
-        <v>100.4958231707317</v>
+        <v>98.47869918699186</v>
       </c>
       <c r="L7">
-        <v>113.29875</v>
+        <v>116.2415989159892</v>
       </c>
       <c r="M7">
-        <v>115.0175</v>
+        <v>114.1211382113821</v>
       </c>
       <c r="N7">
-        <v>75.95158536585365</v>
+        <v>75.78130081300812</v>
       </c>
       <c r="O7">
-        <v>0.353910975609756</v>
+        <v>0.4208696476964769</v>
       </c>
       <c r="P7">
-        <v>0.5622545731707318</v>
+        <v>0.5928539295392954</v>
       </c>
       <c r="Q7">
-        <v>0.2565567073170731</v>
+        <v>0.2782558265582655</v>
       </c>
       <c r="R7">
-        <v>12.55484756097561</v>
+        <v>12.74181571815718</v>
       </c>
       <c r="S7">
-        <v>12.25079268292683</v>
+        <v>12.66457994579946</v>
       </c>
       <c r="T7">
-        <v>0.1932905487804878</v>
+        <v>0.2212917344173442</v>
       </c>
       <c r="U7">
-        <v>1.003509580350636</v>
+        <v>1.014518512173708</v>
       </c>
       <c r="V7">
-        <v>1.046319236921261</v>
+        <v>1.054046745699216</v>
       </c>
       <c r="W7">
-        <v>11.35277984872319</v>
+        <v>11.09933817476387</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -996,129 +990,61 @@
         <v>226.5</v>
       </c>
       <c r="E8">
-        <v>6049076.5</v>
+        <v>8826403</v>
       </c>
       <c r="F8">
-        <v>114.9244047619048</v>
+        <v>112.1877481565513</v>
       </c>
       <c r="G8">
-        <v>14</v>
+        <v>1.5</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J8">
-        <v>0.4817073170731707</v>
+        <v>0.4970184853905784</v>
       </c>
       <c r="K8">
-        <v>97.29541666666665</v>
+        <v>96.1698241633579</v>
       </c>
       <c r="L8">
-        <v>117.3911904761905</v>
+        <v>115.3927963698241</v>
       </c>
       <c r="M8">
-        <v>114.871369047619</v>
+        <v>114.9619965967102</v>
       </c>
       <c r="N8">
-        <v>76.4417261904762</v>
+        <v>76.35748723766307</v>
       </c>
       <c r="O8">
-        <v>0.3649839285714286</v>
+        <v>0.4442799205899035</v>
       </c>
       <c r="P8">
-        <v>0.590007142857143</v>
+        <v>0.5913408961996598</v>
       </c>
       <c r="Q8">
-        <v>0.2486589285714286</v>
+        <v>0.312515598411798</v>
       </c>
       <c r="R8">
-        <v>12.44607142857143</v>
+        <v>12.41948383437323</v>
       </c>
       <c r="S8">
-        <v>12.24357142857143</v>
+        <v>12.01976744186047</v>
       </c>
       <c r="T8">
-        <v>0.2096875000000001</v>
+        <v>0.2289780204197391</v>
       </c>
       <c r="U8">
-        <v>1.009880533935894</v>
+        <v>0.9849670601979924</v>
       </c>
       <c r="V8">
-        <v>0.991124236836904</v>
+        <v>0.9700934153339833</v>
       </c>
       <c r="W8">
-        <v>11.34684067436913</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>2023</v>
-      </c>
-      <c r="D9">
-        <v>236.5</v>
-      </c>
-      <c r="E9">
-        <v>18084349.5</v>
-      </c>
-      <c r="F9">
-        <v>113.9349358974359</v>
-      </c>
-      <c r="G9">
-        <v>9</v>
-      </c>
-      <c r="H9" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9">
-        <v>0.4743421052631579</v>
-      </c>
-      <c r="K9">
-        <v>99.6941346153846</v>
-      </c>
-      <c r="L9">
-        <v>113.7744871794872</v>
-      </c>
-      <c r="M9">
-        <v>116.4991666666667</v>
-      </c>
-      <c r="N9">
-        <v>76.89932692307693</v>
-      </c>
-      <c r="O9">
-        <v>0.4110048076923076</v>
-      </c>
-      <c r="P9">
-        <v>0.5767176282051283</v>
-      </c>
-      <c r="Q9">
-        <v>0.2881881410256409</v>
-      </c>
-      <c r="R9">
-        <v>13.24182692307692</v>
-      </c>
-      <c r="S9">
-        <v>12.29208333333333</v>
-      </c>
-      <c r="T9">
-        <v>0.2205663461538462</v>
-      </c>
-      <c r="U9">
-        <v>1.00118572844847</v>
-      </c>
-      <c r="V9">
-        <v>1.028856924773938</v>
-      </c>
-      <c r="W9">
-        <v>11.25332596191566</v>
+        <v>11.71921768868253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>